<commit_message>
Report + Code Quality
- Code commenting and quality improvements, some more linting to gp
- Need to finish modifying Inpainter.py

- Generating/ Producing images and finished writing report, need to cut down 530 words
</commit_message>
<xml_diff>
--- a/report_assets/accuracy-per-step.xlsx
+++ b/report_assets/accuracy-per-step.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesduxbury/Documents/GitHub/image-processing-coursework/report_assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E994651-5748-294D-A41C-E19A7C3468C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B7FD8D-3151-E143-A6F2-33670F9651D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{F627235B-C503-0745-929E-8043D58A67BE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{F627235B-C503-0745-929E-8043D58A67BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
-  <si>
-    <t>Step</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Technique</t>
   </si>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t>Intermediate Accuracy</t>
-  </si>
-  <si>
-    <t>Final Accuracy Without</t>
   </si>
 </sst>
 </file>
@@ -456,148 +450,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597783E6-6894-D242-92EB-F94A8CB97498}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.69</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>0.52</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="B4" s="1">
         <v>0.52</v>
       </c>
-      <c r="D3" s="1">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.83</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="B5" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="B9" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="B10" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
+      <c r="B11" s="1">
+        <v>0.9</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>